<commit_message>
Add Contracts module and other features
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zulla\Desktop\Beeah Cms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636870D6-171C-4268-9ABD-357788E06AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40411D4A-D1F8-4FC3-A133-4081504C4FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -224,12 +224,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,18 +529,19 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F23" sqref="F21:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -554,336 +571,416 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>14605</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>14606</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>14607</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>14608</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>14609</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>14605</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F23" t="s">
-        <v>25</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>